<commit_message>
Version final final, junto con las pruebas de imagen
</commit_message>
<xml_diff>
--- a/ventas_ingresadas.xlsx
+++ b/ventas_ingresadas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\estadistica_agendamientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositorios\estadistica_agendamientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146BD835-1FFD-496E-9083-F98A085C88A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6B518B-998B-48A2-B658-F69C26FE02D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -376,14 +376,14 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -417,7 +417,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -434,7 +434,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -451,7 +451,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>

</xml_diff>